<commit_message>
Version 1.0.3.5: improved error handling included log4net for message logging
</commit_message>
<xml_diff>
--- a/SAP_AccDoc_1-0-3.xlsx
+++ b/SAP_AccDoc_1-0-3.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VS_WS\SapAccExcelAddin\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\hmun\VbaGit_64\VS_WS\SapAccExcelAddin\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18E5F3E1-EFAB-4F52-B633-106E1371F981}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3135" yWindow="1215" windowWidth="12225" windowHeight="6780" tabRatio="383" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="12390" tabRatio="521" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameter" sheetId="3" r:id="rId1"/>
@@ -32,17 +33,24 @@
     <definedName name="TESTKEYS">'SAP-Acc-Data'!#REF!</definedName>
     <definedName name="TESTVKEY">'SAP-Acc-Data'!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511" refMode="R1C1"/>
+  <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Hermann Mundprecht</author>
   </authors>
   <commentList>
-    <comment ref="N1" authorId="0" shapeId="0">
+    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -66,7 +74,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AM1" authorId="0" shapeId="0">
+    <comment ref="AM1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -95,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="151">
   <si>
     <t>Paramter</t>
   </si>
@@ -547,16 +555,13 @@
     <t>080</t>
   </si>
   <si>
-    <t>Beleg erfolgreich gebucht: BKPFF 001800000302002019 GTMCLNT060</t>
-  </si>
-  <si>
-    <t>001800000302002019</t>
+    <t>001872048702002019</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="_-[$€]\ * #,##0.00_-;\-[$€]\ * #,##0.00_-;_-[$€]\ * \-??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="0000"/>
@@ -2304,174 +2309,174 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="168">
-    <cellStyle name="Accent1 - 20%" xfId="44"/>
-    <cellStyle name="Accent1 - 40%" xfId="45"/>
-    <cellStyle name="Accent1 - 60%" xfId="46"/>
-    <cellStyle name="Accent1 2" xfId="43"/>
-    <cellStyle name="Accent1 3" xfId="122"/>
-    <cellStyle name="Accent1 4" xfId="128"/>
-    <cellStyle name="Accent2 - 20%" xfId="48"/>
-    <cellStyle name="Accent2 - 40%" xfId="49"/>
-    <cellStyle name="Accent2 - 60%" xfId="50"/>
-    <cellStyle name="Accent2 2" xfId="47"/>
-    <cellStyle name="Accent2 3" xfId="123"/>
-    <cellStyle name="Accent2 4" xfId="129"/>
-    <cellStyle name="Accent3 - 20%" xfId="52"/>
-    <cellStyle name="Accent3 - 40%" xfId="53"/>
-    <cellStyle name="Accent3 - 60%" xfId="54"/>
-    <cellStyle name="Accent3 2" xfId="51"/>
-    <cellStyle name="Accent3 3" xfId="124"/>
-    <cellStyle name="Accent3 4" xfId="130"/>
-    <cellStyle name="Accent4 - 20%" xfId="56"/>
-    <cellStyle name="Accent4 - 40%" xfId="57"/>
-    <cellStyle name="Accent4 - 60%" xfId="58"/>
-    <cellStyle name="Accent4 2" xfId="55"/>
-    <cellStyle name="Accent4 3" xfId="125"/>
-    <cellStyle name="Accent4 4" xfId="131"/>
-    <cellStyle name="Accent5 - 20%" xfId="60"/>
-    <cellStyle name="Accent5 - 40%" xfId="61"/>
-    <cellStyle name="Accent5 - 60%" xfId="62"/>
-    <cellStyle name="Accent5 2" xfId="59"/>
-    <cellStyle name="Accent5 3" xfId="126"/>
-    <cellStyle name="Accent5 4" xfId="132"/>
-    <cellStyle name="Accent6 - 20%" xfId="64"/>
-    <cellStyle name="Accent6 - 40%" xfId="65"/>
-    <cellStyle name="Accent6 - 60%" xfId="66"/>
-    <cellStyle name="Accent6 2" xfId="63"/>
-    <cellStyle name="Accent6 3" xfId="127"/>
-    <cellStyle name="Accent6 4" xfId="133"/>
-    <cellStyle name="Bad 2" xfId="67"/>
-    <cellStyle name="Calculation 2" xfId="68"/>
-    <cellStyle name="Check Cell 2" xfId="69"/>
-    <cellStyle name="Emphasis 1" xfId="70"/>
-    <cellStyle name="Emphasis 2" xfId="71"/>
-    <cellStyle name="Emphasis 3" xfId="72"/>
-    <cellStyle name="Euro" xfId="1"/>
-    <cellStyle name="Good 2" xfId="73"/>
-    <cellStyle name="Heading 1 2" xfId="74"/>
-    <cellStyle name="Heading 2 2" xfId="75"/>
-    <cellStyle name="Heading 3 2" xfId="76"/>
-    <cellStyle name="Heading 4 2" xfId="77"/>
-    <cellStyle name="Input 2" xfId="78"/>
-    <cellStyle name="Linked Cell 2" xfId="79"/>
-    <cellStyle name="Neutral 2" xfId="80"/>
+    <cellStyle name="Accent1 - 20%" xfId="44" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Accent1 - 40%" xfId="45" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Accent1 - 60%" xfId="46" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Accent1 2" xfId="43" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Accent1 3" xfId="122" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Accent1 4" xfId="128" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Accent2 - 20%" xfId="48" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Accent2 - 40%" xfId="49" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Accent2 - 60%" xfId="50" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Accent2 2" xfId="47" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Accent2 3" xfId="123" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="Accent2 4" xfId="129" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="Accent3 - 20%" xfId="52" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="Accent3 - 40%" xfId="53" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="Accent3 - 60%" xfId="54" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="Accent3 2" xfId="51" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="Accent3 3" xfId="124" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="Accent3 4" xfId="130" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
+    <cellStyle name="Accent4 - 20%" xfId="56" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
+    <cellStyle name="Accent4 - 40%" xfId="57" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
+    <cellStyle name="Accent4 - 60%" xfId="58" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
+    <cellStyle name="Accent4 2" xfId="55" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
+    <cellStyle name="Accent4 3" xfId="125" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
+    <cellStyle name="Accent4 4" xfId="131" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
+    <cellStyle name="Accent5 - 20%" xfId="60" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
+    <cellStyle name="Accent5 - 40%" xfId="61" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
+    <cellStyle name="Accent5 - 60%" xfId="62" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
+    <cellStyle name="Accent5 2" xfId="59" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
+    <cellStyle name="Accent5 3" xfId="126" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
+    <cellStyle name="Accent5 4" xfId="132" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
+    <cellStyle name="Accent6 - 20%" xfId="64" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
+    <cellStyle name="Accent6 - 40%" xfId="65" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
+    <cellStyle name="Accent6 - 60%" xfId="66" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
+    <cellStyle name="Accent6 2" xfId="63" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
+    <cellStyle name="Accent6 3" xfId="127" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
+    <cellStyle name="Accent6 4" xfId="133" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
+    <cellStyle name="Bad 2" xfId="67" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
+    <cellStyle name="Calculation 2" xfId="68" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
+    <cellStyle name="Check Cell 2" xfId="69" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
+    <cellStyle name="Emphasis 1" xfId="70" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
+    <cellStyle name="Emphasis 2" xfId="71" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
+    <cellStyle name="Emphasis 3" xfId="72" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
+    <cellStyle name="Euro" xfId="1" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
+    <cellStyle name="Good 2" xfId="73" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
+    <cellStyle name="Heading 1 2" xfId="74" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
+    <cellStyle name="Heading 2 2" xfId="75" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
+    <cellStyle name="Heading 3 2" xfId="76" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
+    <cellStyle name="Heading 4 2" xfId="77" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
+    <cellStyle name="Input 2" xfId="78" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
+    <cellStyle name="Linked Cell 2" xfId="79" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
+    <cellStyle name="Neutral 2" xfId="80" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="42"/>
-    <cellStyle name="Note 2" xfId="81"/>
-    <cellStyle name="Output 2" xfId="82"/>
-    <cellStyle name="SAPBEXaggData" xfId="6"/>
-    <cellStyle name="SAPBEXaggDataEmph" xfId="7"/>
-    <cellStyle name="SAPBEXaggDataEmph 2" xfId="83"/>
-    <cellStyle name="SAPBEXaggItem" xfId="8"/>
-    <cellStyle name="SAPBEXaggItem 2" xfId="84"/>
-    <cellStyle name="SAPBEXaggItemX" xfId="9"/>
-    <cellStyle name="SAPBEXaggItemX 2" xfId="85"/>
-    <cellStyle name="SAPBEXchaText" xfId="3"/>
-    <cellStyle name="SAPBEXexcBad7" xfId="10"/>
-    <cellStyle name="SAPBEXexcBad7 2" xfId="86"/>
-    <cellStyle name="SAPBEXexcBad8" xfId="11"/>
-    <cellStyle name="SAPBEXexcBad8 2" xfId="87"/>
-    <cellStyle name="SAPBEXexcBad9" xfId="12"/>
-    <cellStyle name="SAPBEXexcBad9 2" xfId="88"/>
-    <cellStyle name="SAPBEXexcCritical4" xfId="13"/>
-    <cellStyle name="SAPBEXexcCritical4 2" xfId="89"/>
-    <cellStyle name="SAPBEXexcCritical5" xfId="14"/>
-    <cellStyle name="SAPBEXexcCritical5 2" xfId="90"/>
-    <cellStyle name="SAPBEXexcCritical6" xfId="15"/>
-    <cellStyle name="SAPBEXexcCritical6 2" xfId="91"/>
-    <cellStyle name="SAPBEXexcGood1" xfId="16"/>
-    <cellStyle name="SAPBEXexcGood1 2" xfId="92"/>
-    <cellStyle name="SAPBEXexcGood2" xfId="17"/>
-    <cellStyle name="SAPBEXexcGood2 2" xfId="93"/>
-    <cellStyle name="SAPBEXexcGood3" xfId="18"/>
-    <cellStyle name="SAPBEXexcGood3 2" xfId="94"/>
-    <cellStyle name="SAPBEXfilterDrill" xfId="19"/>
-    <cellStyle name="SAPBEXfilterDrill 2" xfId="95"/>
-    <cellStyle name="SAPBEXfilterItem" xfId="20"/>
-    <cellStyle name="SAPBEXfilterItem 2" xfId="96"/>
-    <cellStyle name="SAPBEXfilterText" xfId="21"/>
-    <cellStyle name="SAPBEXfilterText 2" xfId="97"/>
-    <cellStyle name="SAPBEXformats" xfId="5"/>
-    <cellStyle name="SAPBEXheaderItem" xfId="22"/>
-    <cellStyle name="SAPBEXheaderItem 2" xfId="98"/>
-    <cellStyle name="SAPBEXheaderText" xfId="23"/>
-    <cellStyle name="SAPBEXheaderText 2" xfId="99"/>
-    <cellStyle name="SAPBEXHLevel0" xfId="24"/>
-    <cellStyle name="SAPBEXHLevel0 2" xfId="100"/>
-    <cellStyle name="SAPBEXHLevel0X" xfId="25"/>
-    <cellStyle name="SAPBEXHLevel0X 2" xfId="101"/>
-    <cellStyle name="SAPBEXHLevel1" xfId="26"/>
-    <cellStyle name="SAPBEXHLevel1 2" xfId="102"/>
-    <cellStyle name="SAPBEXHLevel1X" xfId="27"/>
-    <cellStyle name="SAPBEXHLevel1X 2" xfId="103"/>
-    <cellStyle name="SAPBEXHLevel2" xfId="28"/>
-    <cellStyle name="SAPBEXHLevel2 2" xfId="104"/>
-    <cellStyle name="SAPBEXHLevel2X" xfId="29"/>
-    <cellStyle name="SAPBEXHLevel2X 2" xfId="105"/>
-    <cellStyle name="SAPBEXHLevel3" xfId="30"/>
-    <cellStyle name="SAPBEXHLevel3 2" xfId="106"/>
-    <cellStyle name="SAPBEXHLevel3X" xfId="31"/>
-    <cellStyle name="SAPBEXHLevel3X 2" xfId="107"/>
-    <cellStyle name="SAPBEXinputData" xfId="32"/>
-    <cellStyle name="SAPBEXinputData 2" xfId="108"/>
-    <cellStyle name="SAPBEXItemHeader" xfId="109"/>
-    <cellStyle name="SAPBEXresData" xfId="33"/>
-    <cellStyle name="SAPBEXresData 2" xfId="110"/>
-    <cellStyle name="SAPBEXresDataEmph" xfId="34"/>
-    <cellStyle name="SAPBEXresDataEmph 2" xfId="111"/>
-    <cellStyle name="SAPBEXresItem" xfId="35"/>
-    <cellStyle name="SAPBEXresItem 2" xfId="112"/>
-    <cellStyle name="SAPBEXresItemX" xfId="36"/>
-    <cellStyle name="SAPBEXresItemX 2" xfId="113"/>
-    <cellStyle name="SAPBEXstdData" xfId="2"/>
-    <cellStyle name="SAPBEXstdDataEmph" xfId="37"/>
-    <cellStyle name="SAPBEXstdDataEmph 2" xfId="114"/>
-    <cellStyle name="SAPBEXstdItem" xfId="4"/>
-    <cellStyle name="SAPBEXstdItemX" xfId="38"/>
-    <cellStyle name="SAPBEXstdItemX 2" xfId="115"/>
-    <cellStyle name="SAPBEXtitle" xfId="39"/>
-    <cellStyle name="SAPBEXtitle 2" xfId="116"/>
-    <cellStyle name="SAPBEXunassignedItem" xfId="117"/>
-    <cellStyle name="SAPBEXundefined" xfId="40"/>
-    <cellStyle name="SAPBEXundefined 2" xfId="118"/>
-    <cellStyle name="SAPBorder" xfId="152"/>
-    <cellStyle name="SAPDataCell" xfId="135"/>
-    <cellStyle name="SAPDataTotalCell" xfId="136"/>
-    <cellStyle name="SAPDimensionCell" xfId="134"/>
-    <cellStyle name="SAPEditableDataCell" xfId="137"/>
-    <cellStyle name="SAPEditableDataTotalCell" xfId="140"/>
-    <cellStyle name="SAPEmphasized" xfId="160"/>
-    <cellStyle name="SAPEmphasizedEditableDataCell" xfId="162"/>
-    <cellStyle name="SAPEmphasizedEditableDataTotalCell" xfId="163"/>
-    <cellStyle name="SAPEmphasizedLockedDataCell" xfId="166"/>
-    <cellStyle name="SAPEmphasizedLockedDataTotalCell" xfId="167"/>
-    <cellStyle name="SAPEmphasizedReadonlyDataCell" xfId="164"/>
-    <cellStyle name="SAPEmphasizedReadonlyDataTotalCell" xfId="165"/>
-    <cellStyle name="SAPEmphasizedTotal" xfId="161"/>
-    <cellStyle name="SAPExceptionLevel1" xfId="143"/>
-    <cellStyle name="SAPExceptionLevel2" xfId="144"/>
-    <cellStyle name="SAPExceptionLevel3" xfId="145"/>
-    <cellStyle name="SAPExceptionLevel4" xfId="146"/>
-    <cellStyle name="SAPExceptionLevel5" xfId="147"/>
-    <cellStyle name="SAPExceptionLevel6" xfId="148"/>
-    <cellStyle name="SAPExceptionLevel7" xfId="149"/>
-    <cellStyle name="SAPExceptionLevel8" xfId="150"/>
-    <cellStyle name="SAPExceptionLevel9" xfId="151"/>
-    <cellStyle name="SAPHierarchyCell0" xfId="155"/>
-    <cellStyle name="SAPHierarchyCell1" xfId="156"/>
-    <cellStyle name="SAPHierarchyCell2" xfId="157"/>
-    <cellStyle name="SAPHierarchyCell3" xfId="158"/>
-    <cellStyle name="SAPHierarchyCell4" xfId="159"/>
-    <cellStyle name="SAPLockedDataCell" xfId="139"/>
-    <cellStyle name="SAPLockedDataTotalCell" xfId="142"/>
-    <cellStyle name="SAPMemberCell" xfId="153"/>
-    <cellStyle name="SAPMemberTotalCell" xfId="154"/>
-    <cellStyle name="SAPReadonlyDataCell" xfId="138"/>
-    <cellStyle name="SAPReadonlyDataTotalCell" xfId="141"/>
-    <cellStyle name="Sheet Title" xfId="119"/>
-    <cellStyle name="Standard 2" xfId="41"/>
-    <cellStyle name="Total 2" xfId="120"/>
-    <cellStyle name="Warning Text 2" xfId="121"/>
+    <cellStyle name="Normal 2" xfId="42" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
+    <cellStyle name="Note 2" xfId="81" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
+    <cellStyle name="Output 2" xfId="82" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
+    <cellStyle name="SAPBEXaggData" xfId="6" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
+    <cellStyle name="SAPBEXaggDataEmph" xfId="7" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
+    <cellStyle name="SAPBEXaggDataEmph 2" xfId="83" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
+    <cellStyle name="SAPBEXaggItem" xfId="8" xr:uid="{00000000-0005-0000-0000-00003A000000}"/>
+    <cellStyle name="SAPBEXaggItem 2" xfId="84" xr:uid="{00000000-0005-0000-0000-00003B000000}"/>
+    <cellStyle name="SAPBEXaggItemX" xfId="9" xr:uid="{00000000-0005-0000-0000-00003C000000}"/>
+    <cellStyle name="SAPBEXaggItemX 2" xfId="85" xr:uid="{00000000-0005-0000-0000-00003D000000}"/>
+    <cellStyle name="SAPBEXchaText" xfId="3" xr:uid="{00000000-0005-0000-0000-00003E000000}"/>
+    <cellStyle name="SAPBEXexcBad7" xfId="10" xr:uid="{00000000-0005-0000-0000-00003F000000}"/>
+    <cellStyle name="SAPBEXexcBad7 2" xfId="86" xr:uid="{00000000-0005-0000-0000-000040000000}"/>
+    <cellStyle name="SAPBEXexcBad8" xfId="11" xr:uid="{00000000-0005-0000-0000-000041000000}"/>
+    <cellStyle name="SAPBEXexcBad8 2" xfId="87" xr:uid="{00000000-0005-0000-0000-000042000000}"/>
+    <cellStyle name="SAPBEXexcBad9" xfId="12" xr:uid="{00000000-0005-0000-0000-000043000000}"/>
+    <cellStyle name="SAPBEXexcBad9 2" xfId="88" xr:uid="{00000000-0005-0000-0000-000044000000}"/>
+    <cellStyle name="SAPBEXexcCritical4" xfId="13" xr:uid="{00000000-0005-0000-0000-000045000000}"/>
+    <cellStyle name="SAPBEXexcCritical4 2" xfId="89" xr:uid="{00000000-0005-0000-0000-000046000000}"/>
+    <cellStyle name="SAPBEXexcCritical5" xfId="14" xr:uid="{00000000-0005-0000-0000-000047000000}"/>
+    <cellStyle name="SAPBEXexcCritical5 2" xfId="90" xr:uid="{00000000-0005-0000-0000-000048000000}"/>
+    <cellStyle name="SAPBEXexcCritical6" xfId="15" xr:uid="{00000000-0005-0000-0000-000049000000}"/>
+    <cellStyle name="SAPBEXexcCritical6 2" xfId="91" xr:uid="{00000000-0005-0000-0000-00004A000000}"/>
+    <cellStyle name="SAPBEXexcGood1" xfId="16" xr:uid="{00000000-0005-0000-0000-00004B000000}"/>
+    <cellStyle name="SAPBEXexcGood1 2" xfId="92" xr:uid="{00000000-0005-0000-0000-00004C000000}"/>
+    <cellStyle name="SAPBEXexcGood2" xfId="17" xr:uid="{00000000-0005-0000-0000-00004D000000}"/>
+    <cellStyle name="SAPBEXexcGood2 2" xfId="93" xr:uid="{00000000-0005-0000-0000-00004E000000}"/>
+    <cellStyle name="SAPBEXexcGood3" xfId="18" xr:uid="{00000000-0005-0000-0000-00004F000000}"/>
+    <cellStyle name="SAPBEXexcGood3 2" xfId="94" xr:uid="{00000000-0005-0000-0000-000050000000}"/>
+    <cellStyle name="SAPBEXfilterDrill" xfId="19" xr:uid="{00000000-0005-0000-0000-000051000000}"/>
+    <cellStyle name="SAPBEXfilterDrill 2" xfId="95" xr:uid="{00000000-0005-0000-0000-000052000000}"/>
+    <cellStyle name="SAPBEXfilterItem" xfId="20" xr:uid="{00000000-0005-0000-0000-000053000000}"/>
+    <cellStyle name="SAPBEXfilterItem 2" xfId="96" xr:uid="{00000000-0005-0000-0000-000054000000}"/>
+    <cellStyle name="SAPBEXfilterText" xfId="21" xr:uid="{00000000-0005-0000-0000-000055000000}"/>
+    <cellStyle name="SAPBEXfilterText 2" xfId="97" xr:uid="{00000000-0005-0000-0000-000056000000}"/>
+    <cellStyle name="SAPBEXformats" xfId="5" xr:uid="{00000000-0005-0000-0000-000057000000}"/>
+    <cellStyle name="SAPBEXheaderItem" xfId="22" xr:uid="{00000000-0005-0000-0000-000058000000}"/>
+    <cellStyle name="SAPBEXheaderItem 2" xfId="98" xr:uid="{00000000-0005-0000-0000-000059000000}"/>
+    <cellStyle name="SAPBEXheaderText" xfId="23" xr:uid="{00000000-0005-0000-0000-00005A000000}"/>
+    <cellStyle name="SAPBEXheaderText 2" xfId="99" xr:uid="{00000000-0005-0000-0000-00005B000000}"/>
+    <cellStyle name="SAPBEXHLevel0" xfId="24" xr:uid="{00000000-0005-0000-0000-00005C000000}"/>
+    <cellStyle name="SAPBEXHLevel0 2" xfId="100" xr:uid="{00000000-0005-0000-0000-00005D000000}"/>
+    <cellStyle name="SAPBEXHLevel0X" xfId="25" xr:uid="{00000000-0005-0000-0000-00005E000000}"/>
+    <cellStyle name="SAPBEXHLevel0X 2" xfId="101" xr:uid="{00000000-0005-0000-0000-00005F000000}"/>
+    <cellStyle name="SAPBEXHLevel1" xfId="26" xr:uid="{00000000-0005-0000-0000-000060000000}"/>
+    <cellStyle name="SAPBEXHLevel1 2" xfId="102" xr:uid="{00000000-0005-0000-0000-000061000000}"/>
+    <cellStyle name="SAPBEXHLevel1X" xfId="27" xr:uid="{00000000-0005-0000-0000-000062000000}"/>
+    <cellStyle name="SAPBEXHLevel1X 2" xfId="103" xr:uid="{00000000-0005-0000-0000-000063000000}"/>
+    <cellStyle name="SAPBEXHLevel2" xfId="28" xr:uid="{00000000-0005-0000-0000-000064000000}"/>
+    <cellStyle name="SAPBEXHLevel2 2" xfId="104" xr:uid="{00000000-0005-0000-0000-000065000000}"/>
+    <cellStyle name="SAPBEXHLevel2X" xfId="29" xr:uid="{00000000-0005-0000-0000-000066000000}"/>
+    <cellStyle name="SAPBEXHLevel2X 2" xfId="105" xr:uid="{00000000-0005-0000-0000-000067000000}"/>
+    <cellStyle name="SAPBEXHLevel3" xfId="30" xr:uid="{00000000-0005-0000-0000-000068000000}"/>
+    <cellStyle name="SAPBEXHLevel3 2" xfId="106" xr:uid="{00000000-0005-0000-0000-000069000000}"/>
+    <cellStyle name="SAPBEXHLevel3X" xfId="31" xr:uid="{00000000-0005-0000-0000-00006A000000}"/>
+    <cellStyle name="SAPBEXHLevel3X 2" xfId="107" xr:uid="{00000000-0005-0000-0000-00006B000000}"/>
+    <cellStyle name="SAPBEXinputData" xfId="32" xr:uid="{00000000-0005-0000-0000-00006C000000}"/>
+    <cellStyle name="SAPBEXinputData 2" xfId="108" xr:uid="{00000000-0005-0000-0000-00006D000000}"/>
+    <cellStyle name="SAPBEXItemHeader" xfId="109" xr:uid="{00000000-0005-0000-0000-00006E000000}"/>
+    <cellStyle name="SAPBEXresData" xfId="33" xr:uid="{00000000-0005-0000-0000-00006F000000}"/>
+    <cellStyle name="SAPBEXresData 2" xfId="110" xr:uid="{00000000-0005-0000-0000-000070000000}"/>
+    <cellStyle name="SAPBEXresDataEmph" xfId="34" xr:uid="{00000000-0005-0000-0000-000071000000}"/>
+    <cellStyle name="SAPBEXresDataEmph 2" xfId="111" xr:uid="{00000000-0005-0000-0000-000072000000}"/>
+    <cellStyle name="SAPBEXresItem" xfId="35" xr:uid="{00000000-0005-0000-0000-000073000000}"/>
+    <cellStyle name="SAPBEXresItem 2" xfId="112" xr:uid="{00000000-0005-0000-0000-000074000000}"/>
+    <cellStyle name="SAPBEXresItemX" xfId="36" xr:uid="{00000000-0005-0000-0000-000075000000}"/>
+    <cellStyle name="SAPBEXresItemX 2" xfId="113" xr:uid="{00000000-0005-0000-0000-000076000000}"/>
+    <cellStyle name="SAPBEXstdData" xfId="2" xr:uid="{00000000-0005-0000-0000-000077000000}"/>
+    <cellStyle name="SAPBEXstdDataEmph" xfId="37" xr:uid="{00000000-0005-0000-0000-000078000000}"/>
+    <cellStyle name="SAPBEXstdDataEmph 2" xfId="114" xr:uid="{00000000-0005-0000-0000-000079000000}"/>
+    <cellStyle name="SAPBEXstdItem" xfId="4" xr:uid="{00000000-0005-0000-0000-00007A000000}"/>
+    <cellStyle name="SAPBEXstdItemX" xfId="38" xr:uid="{00000000-0005-0000-0000-00007B000000}"/>
+    <cellStyle name="SAPBEXstdItemX 2" xfId="115" xr:uid="{00000000-0005-0000-0000-00007C000000}"/>
+    <cellStyle name="SAPBEXtitle" xfId="39" xr:uid="{00000000-0005-0000-0000-00007D000000}"/>
+    <cellStyle name="SAPBEXtitle 2" xfId="116" xr:uid="{00000000-0005-0000-0000-00007E000000}"/>
+    <cellStyle name="SAPBEXunassignedItem" xfId="117" xr:uid="{00000000-0005-0000-0000-00007F000000}"/>
+    <cellStyle name="SAPBEXundefined" xfId="40" xr:uid="{00000000-0005-0000-0000-000080000000}"/>
+    <cellStyle name="SAPBEXundefined 2" xfId="118" xr:uid="{00000000-0005-0000-0000-000081000000}"/>
+    <cellStyle name="SAPBorder" xfId="152" xr:uid="{00000000-0005-0000-0000-000082000000}"/>
+    <cellStyle name="SAPDataCell" xfId="135" xr:uid="{00000000-0005-0000-0000-000083000000}"/>
+    <cellStyle name="SAPDataTotalCell" xfId="136" xr:uid="{00000000-0005-0000-0000-000084000000}"/>
+    <cellStyle name="SAPDimensionCell" xfId="134" xr:uid="{00000000-0005-0000-0000-000085000000}"/>
+    <cellStyle name="SAPEditableDataCell" xfId="137" xr:uid="{00000000-0005-0000-0000-000086000000}"/>
+    <cellStyle name="SAPEditableDataTotalCell" xfId="140" xr:uid="{00000000-0005-0000-0000-000087000000}"/>
+    <cellStyle name="SAPEmphasized" xfId="160" xr:uid="{00000000-0005-0000-0000-000088000000}"/>
+    <cellStyle name="SAPEmphasizedEditableDataCell" xfId="162" xr:uid="{00000000-0005-0000-0000-000089000000}"/>
+    <cellStyle name="SAPEmphasizedEditableDataTotalCell" xfId="163" xr:uid="{00000000-0005-0000-0000-00008A000000}"/>
+    <cellStyle name="SAPEmphasizedLockedDataCell" xfId="166" xr:uid="{00000000-0005-0000-0000-00008B000000}"/>
+    <cellStyle name="SAPEmphasizedLockedDataTotalCell" xfId="167" xr:uid="{00000000-0005-0000-0000-00008C000000}"/>
+    <cellStyle name="SAPEmphasizedReadonlyDataCell" xfId="164" xr:uid="{00000000-0005-0000-0000-00008D000000}"/>
+    <cellStyle name="SAPEmphasizedReadonlyDataTotalCell" xfId="165" xr:uid="{00000000-0005-0000-0000-00008E000000}"/>
+    <cellStyle name="SAPEmphasizedTotal" xfId="161" xr:uid="{00000000-0005-0000-0000-00008F000000}"/>
+    <cellStyle name="SAPExceptionLevel1" xfId="143" xr:uid="{00000000-0005-0000-0000-000090000000}"/>
+    <cellStyle name="SAPExceptionLevel2" xfId="144" xr:uid="{00000000-0005-0000-0000-000091000000}"/>
+    <cellStyle name="SAPExceptionLevel3" xfId="145" xr:uid="{00000000-0005-0000-0000-000092000000}"/>
+    <cellStyle name="SAPExceptionLevel4" xfId="146" xr:uid="{00000000-0005-0000-0000-000093000000}"/>
+    <cellStyle name="SAPExceptionLevel5" xfId="147" xr:uid="{00000000-0005-0000-0000-000094000000}"/>
+    <cellStyle name="SAPExceptionLevel6" xfId="148" xr:uid="{00000000-0005-0000-0000-000095000000}"/>
+    <cellStyle name="SAPExceptionLevel7" xfId="149" xr:uid="{00000000-0005-0000-0000-000096000000}"/>
+    <cellStyle name="SAPExceptionLevel8" xfId="150" xr:uid="{00000000-0005-0000-0000-000097000000}"/>
+    <cellStyle name="SAPExceptionLevel9" xfId="151" xr:uid="{00000000-0005-0000-0000-000098000000}"/>
+    <cellStyle name="SAPHierarchyCell0" xfId="155" xr:uid="{00000000-0005-0000-0000-000099000000}"/>
+    <cellStyle name="SAPHierarchyCell1" xfId="156" xr:uid="{00000000-0005-0000-0000-00009A000000}"/>
+    <cellStyle name="SAPHierarchyCell2" xfId="157" xr:uid="{00000000-0005-0000-0000-00009B000000}"/>
+    <cellStyle name="SAPHierarchyCell3" xfId="158" xr:uid="{00000000-0005-0000-0000-00009C000000}"/>
+    <cellStyle name="SAPHierarchyCell4" xfId="159" xr:uid="{00000000-0005-0000-0000-00009D000000}"/>
+    <cellStyle name="SAPLockedDataCell" xfId="139" xr:uid="{00000000-0005-0000-0000-00009E000000}"/>
+    <cellStyle name="SAPLockedDataTotalCell" xfId="142" xr:uid="{00000000-0005-0000-0000-00009F000000}"/>
+    <cellStyle name="SAPMemberCell" xfId="153" xr:uid="{00000000-0005-0000-0000-0000A0000000}"/>
+    <cellStyle name="SAPMemberTotalCell" xfId="154" xr:uid="{00000000-0005-0000-0000-0000A1000000}"/>
+    <cellStyle name="SAPReadonlyDataCell" xfId="138" xr:uid="{00000000-0005-0000-0000-0000A2000000}"/>
+    <cellStyle name="SAPReadonlyDataTotalCell" xfId="141" xr:uid="{00000000-0005-0000-0000-0000A3000000}"/>
+    <cellStyle name="Sheet Title" xfId="119" xr:uid="{00000000-0005-0000-0000-0000A4000000}"/>
+    <cellStyle name="Standard 2" xfId="41" xr:uid="{00000000-0005-0000-0000-0000A5000000}"/>
+    <cellStyle name="Total 2" xfId="120" xr:uid="{00000000-0005-0000-0000-0000A6000000}"/>
+    <cellStyle name="Warning Text 2" xfId="121" xr:uid="{00000000-0005-0000-0000-0000A7000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -2562,6 +2567,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2597,6 +2619,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2772,7 +2811,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Tabelle3"/>
   <dimension ref="A1:G18"/>
   <sheetViews>
@@ -3037,12 +3076,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:BG21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="BF3" sqref="BF3"/>
@@ -3334,11 +3373,11 @@
         <v>99</v>
       </c>
       <c r="AW3" s="72">
-        <v>43484</v>
+        <v>43748</v>
       </c>
       <c r="AX3" s="72">
         <f>AW3</f>
-        <v>43484</v>
+        <v>43748</v>
       </c>
       <c r="AY3" s="5">
         <v>90000036</v>
@@ -3352,11 +3391,8 @@
       <c r="BC3" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="BF3" s="5" t="s">
+      <c r="BG3" s="40" t="s">
         <v>150</v>
-      </c>
-      <c r="BG3" s="40" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:59" x14ac:dyDescent="0.2">
@@ -3484,12 +3520,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3700,6 +3736,9 @@
       <c r="B16" s="67" t="s">
         <v>129</v>
       </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="59"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Version: 1.0.3.8 - uses SapCommon and SapLogon
</commit_message>
<xml_diff>
--- a/SAP_AccDoc_1-0-3.xlsx
+++ b/SAP_AccDoc_1-0-3.xlsx
@@ -5,17 +5,17 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\hmun\VbaGit_64\VS_WS\SapAccExcelAddin\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\hmun\VbaGit_64\VS_WS (x86)\SapAccExcelAddin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18E5F3E1-EFAB-4F52-B633-106E1371F981}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D049F3BE-F581-4FD5-B846-2A1BBBA5F0CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="12390" tabRatio="521" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="12390" tabRatio="521" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameter" sheetId="3" r:id="rId1"/>
     <sheet name="SAP-Acc-Data" sheetId="4" r:id="rId2"/>
-    <sheet name="SAP-Con" sheetId="8" r:id="rId3"/>
+    <sheet name="SAP-Con" sheetId="8" state="hidden" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_DAT1">'SAP-Acc-Data'!#REF!</definedName>
@@ -33,7 +33,7 @@
     <definedName name="TESTKEYS">'SAP-Acc-Data'!#REF!</definedName>
     <definedName name="TESTVKEY">'SAP-Acc-Data'!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="181029" refMode="R1C1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -555,7 +555,7 @@
     <t>080</t>
   </si>
   <si>
-    <t>001872048702002019</t>
+    <t>$ GTMCLNT060</t>
   </si>
 </sst>
 </file>
@@ -1265,7 +1265,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="45">
+  <borders count="48">
     <border>
       <left/>
       <right/>
@@ -1834,6 +1834,39 @@
         <color indexed="64"/>
       </right>
       <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -2152,7 +2185,7 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2307,6 +2340,10 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="168">
     <cellStyle name="Accent1 - 20%" xfId="44" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -2815,7 +2852,7 @@
   <sheetPr codeName="Tabelle3"/>
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
@@ -3080,7 +3117,7 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:BG21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -3522,165 +3559,174 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="73" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="74"/>
+      <c r="B1" s="80"/>
       <c r="C1" s="74"/>
       <c r="D1" s="74"/>
       <c r="E1" s="74"/>
       <c r="F1" s="74"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" s="74"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="60" t="s">
         <v>91</v>
       </c>
-      <c r="B2" s="61" t="s">
+      <c r="B2" s="81"/>
+      <c r="C2" s="61" t="s">
         <v>102</v>
       </c>
-      <c r="C2" s="61" t="s">
+      <c r="D2" s="61" t="s">
         <v>141</v>
       </c>
-      <c r="D2" s="61" t="s">
+      <c r="E2" s="61" t="s">
         <v>145</v>
       </c>
-      <c r="E2" s="61" t="s">
+      <c r="F2" s="61" t="s">
         <v>113</v>
       </c>
-      <c r="F2" s="61" t="s">
+      <c r="G2" s="61" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="60" t="s">
         <v>132</v>
       </c>
-      <c r="B3" s="61" t="s">
+      <c r="B3" s="81"/>
+      <c r="C3" s="61" t="s">
         <v>100</v>
       </c>
-      <c r="C3" s="61" t="s">
+      <c r="D3" s="61" t="s">
         <v>142</v>
       </c>
-      <c r="D3" s="61" t="s">
+      <c r="E3" s="61" t="s">
         <v>146</v>
       </c>
-      <c r="E3" s="61" t="s">
+      <c r="F3" s="61" t="s">
         <v>110</v>
       </c>
-      <c r="F3" s="61" t="s">
+      <c r="G3" s="61" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="60" t="s">
         <v>133</v>
       </c>
-      <c r="B4" s="79" t="s">
+      <c r="B4" s="81"/>
+      <c r="C4" s="79" t="s">
         <v>137</v>
       </c>
-      <c r="C4" s="79" t="s">
+      <c r="D4" s="79" t="s">
         <v>143</v>
       </c>
-      <c r="D4" s="79" t="s">
+      <c r="E4" s="79" t="s">
         <v>147</v>
-      </c>
-      <c r="E4" s="61" t="s">
-        <v>111</v>
       </c>
       <c r="F4" s="61" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4" s="61" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="60" t="s">
         <v>134</v>
       </c>
-      <c r="B5" s="61" t="s">
+      <c r="B5" s="81"/>
+      <c r="C5" s="61" t="s">
         <v>101</v>
       </c>
-      <c r="C5" s="61" t="s">
+      <c r="D5" s="61" t="s">
         <v>144</v>
       </c>
-      <c r="D5" s="61" t="s">
+      <c r="E5" s="61" t="s">
         <v>148</v>
       </c>
-      <c r="E5" s="61" t="s">
+      <c r="F5" s="61" t="s">
         <v>112</v>
       </c>
-      <c r="F5" s="61" t="s">
+      <c r="G5" s="61" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="60" t="s">
         <v>135</v>
       </c>
-      <c r="B6" s="61"/>
+      <c r="B6" s="81"/>
       <c r="C6" s="61"/>
       <c r="D6" s="61"/>
       <c r="E6" s="61"/>
       <c r="F6" s="61"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G6" s="61"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="60" t="s">
         <v>136</v>
       </c>
-      <c r="B7" s="61"/>
+      <c r="B7" s="81"/>
       <c r="C7" s="61"/>
       <c r="D7" s="61"/>
       <c r="E7" s="61"/>
       <c r="F7" s="61"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7" s="61"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="60" t="s">
         <v>93</v>
       </c>
-      <c r="B8" s="61"/>
+      <c r="B8" s="81"/>
       <c r="C8" s="61"/>
       <c r="D8" s="61"/>
       <c r="E8" s="61"/>
       <c r="F8" s="61"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8" s="61"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="60" t="s">
         <v>94</v>
       </c>
-      <c r="B9" s="68" t="s">
-        <v>103</v>
-      </c>
+      <c r="B9" s="81"/>
       <c r="C9" s="68" t="s">
         <v>103</v>
       </c>
       <c r="D9" s="68" t="s">
+        <v>103</v>
+      </c>
+      <c r="E9" s="68" t="s">
         <v>149</v>
       </c>
-      <c r="E9" s="68" t="s">
+      <c r="F9" s="68" t="s">
         <v>114</v>
       </c>
-      <c r="F9" s="68" t="s">
+      <c r="G9" s="68" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="B10" s="75" t="s">
-        <v>98</v>
-      </c>
+      <c r="B10" s="81"/>
       <c r="C10" s="75" t="s">
         <v>98</v>
       </c>
@@ -3688,40 +3734,45 @@
         <v>98</v>
       </c>
       <c r="E10" s="75" t="s">
-        <v>115</v>
+        <v>98</v>
       </c>
       <c r="F10" s="75" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G10" s="75" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="76" t="s">
         <v>120</v>
       </c>
-      <c r="B11" s="75"/>
+      <c r="B11" s="82"/>
       <c r="C11" s="75"/>
       <c r="D11" s="75"/>
       <c r="E11" s="75"/>
       <c r="F11" s="75"/>
-    </row>
-    <row r="12" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G11" s="75"/>
+    </row>
+    <row r="12" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="66" t="s">
         <v>121</v>
       </c>
-      <c r="B12" s="67"/>
+      <c r="B12" s="83"/>
       <c r="C12" s="67"/>
       <c r="D12" s="67"/>
       <c r="E12" s="67"/>
       <c r="F12" s="67"/>
-    </row>
-    <row r="13" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G12" s="67"/>
+    </row>
+    <row r="13" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="62" t="s">
         <v>95</v>
       </c>
       <c r="B14" s="63"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="64" t="s">
         <v>96</v>
       </c>
@@ -3729,7 +3780,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="66" t="s">
         <v>97</v>
       </c>

</xml_diff>